<commit_message>
formatting+response checks and organisation in place. further functionality available
</commit_message>
<xml_diff>
--- a/Shouvik Guha_health_fitness_tracker.xlsx
+++ b/Shouvik Guha_health_fitness_tracker.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -766,6 +766,28 @@
         </is>
       </c>
       <c r="E12" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2023-12-04 12:16:36</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Gym: Shoulders</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -782,7 +804,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1007,6 +1029,116 @@
       <c r="D10" t="inlineStr">
         <is>
           <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2023-12-04 12:10:04</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>34: 34: 4</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2023-12-04 12:12:02</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2023-12-04 12:12:33</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2023-12-04 12:14:43</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2023-12-04 12:16:23</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1021,7 +1153,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1143,12 +1275,523 @@
         <v>4</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2023-12-04 11:01:54</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Improving Muscle Tone</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2023-12-04 12:16:46</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>83</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Maintaining Current Weight</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>2023-12-02 08:03:05</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>1000-1500</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>1000-1500</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>1000-1500</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2023-12-02 08:03:05</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1000-1500</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1000-1500</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1000-1500</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2023-12-02 08:06:18</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1500-2000</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1000-1500</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>800-1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2023-12-02 08:06:18</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1500-2000</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>1000-1500</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>800-1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2023-12-04 12:16:57</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1500-2000</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2000-2500</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1500-2000</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>2023-12-02 08:03:15</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>2-3</t>
+        </is>
+      </c>
+      <c r="C1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2023-12-02 08:03:15</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2-3</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2023-12-02 08:06:25</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>3-4</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2023-12-02 08:06:25</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>3-4</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2023-12-04 12:17:08</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2-3</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>2023-12-02 08:04:12</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2023-12-02 08:04:12</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2023-12-02 08:06:32</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2023-12-02 08:06:32</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2023-12-04 12:17:15</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>2023-12-02 08:05:09</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>happy, sad</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2023-12-02 08:05:09</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>happy, sad</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2023-12-04 12:17:22</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>cold, tired, sleepy</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1165,420 +1808,84 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>2023-12-02 08:03:05</t>
+          <t>2023-12-02 08:05:24</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>1000-1500</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>1000-1500</t>
+          <t>Yes: Sleep</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>1000-1500</t>
+          <t>finance, personal life</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2023-12-02 08:03:05</t>
+          <t>2023-12-02 08:05:24</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1000-1500</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1000-1500</t>
+          <t>Yes: Sleep</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1000-1500</t>
+          <t>finance, personal life</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2023-12-02 08:06:18</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1500-2000</t>
-        </is>
+          <t>2023-12-04 11:53:49</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>5</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1000-1500</t>
+          <t>Yes: sleep</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>800-1000</t>
+          <t>work, health</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2023-12-02 08:06:18</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1500-2000</t>
-        </is>
+          <t>2023-12-04 12:17:36</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1000-1500</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>800-1000</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>2023-12-02 08:03:15</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>2-3</t>
-        </is>
-      </c>
-      <c r="C1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2023-12-02 08:03:15</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2-3</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D2" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2023-12-02 08:06:25</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>5</v>
-      </c>
-      <c r="D3" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2023-12-02 08:06:25</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>5</v>
-      </c>
-      <c r="D4" t="n">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>2023-12-02 08:04:12</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2023-12-02 08:04:12</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>3</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2023-12-02 08:06:32</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2023-12-02 08:06:32</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>2023-12-02 08:05:09</t>
-        </is>
-      </c>
-      <c r="B1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>happy, sad</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2023-12-02 08:05:09</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>happy, sad</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>2023-12-02 08:05:24</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Yes: Sleep</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>finance, personal life</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2023-12-02 08:05:24</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Yes: Sleep</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>finance, personal life</t>
+          <t>other</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
input checks in place and logic efficiency improved, properly working members. code cleaning still req.
</commit_message>
<xml_diff>
--- a/Shouvik Guha_health_fitness_tracker.xlsx
+++ b/Shouvik Guha_health_fitness_tracker.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -788,6 +788,50 @@
         </is>
       </c>
       <c r="D13" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2023-12-05 07:34:58</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Gym: Core</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2023-12-05 07:52:03</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Gym: Shoulders</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -804,7 +848,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1140,6 +1184,53 @@
         <is>
           <t>3</t>
         </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2023-12-05 07:52:24</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2, 2, 2</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2023-12-06 22:34:11</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>standard</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>3, 3, 3</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1153,7 +1244,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1325,12 +1416,604 @@
         <v>4</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2023-12-05 07:52:51</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Weight Gain</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>2023-12-02 08:03:05</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>1000-1500</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>1000-1500</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>1000-1500</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2023-12-02 08:03:05</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1000-1500</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1000-1500</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1000-1500</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2023-12-02 08:06:18</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1500-2000</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1000-1500</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>800-1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2023-12-02 08:06:18</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1500-2000</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>1000-1500</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>800-1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2023-12-04 12:16:57</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1500-2000</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2000-2500</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1500-2000</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2023-12-05 07:53:00</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2000-2500</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1500-2000</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1500-2000</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>2023-12-02 08:03:15</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>2-3</t>
+        </is>
+      </c>
+      <c r="C1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2023-12-02 08:03:15</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2-3</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2023-12-02 08:06:25</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>3-4</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2023-12-02 08:06:25</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>3-4</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2023-12-04 12:17:08</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2-3</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2023-12-05 07:53:13</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>&gt;4</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>2023-12-02 08:04:12</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2023-12-02 08:04:12</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2023-12-02 08:06:32</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2023-12-02 08:06:32</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2023-12-04 12:17:15</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2023-12-05 07:33:38</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>34</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2023-12-05 07:53:19</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>4</v>
+      </c>
+      <c r="C7" t="n">
+        <v>4</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>2023-12-02 08:05:09</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>happy, sad</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2023-12-02 08:05:09</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>happy, sad</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2023-12-04 12:17:22</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>cold, tired, sleepy</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2023-12-05 07:54:13</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1347,545 +2030,104 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>2023-12-02 08:03:05</t>
+          <t>2023-12-02 08:05:24</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>1000-1500</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>1000-1500</t>
+          <t>Yes: Sleep</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>1000-1500</t>
+          <t>finance, personal life</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2023-12-02 08:03:05</t>
+          <t>2023-12-02 08:05:24</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1000-1500</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1000-1500</t>
+          <t>Yes: Sleep</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1000-1500</t>
+          <t>finance, personal life</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2023-12-02 08:06:18</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1500-2000</t>
-        </is>
+          <t>2023-12-04 11:53:49</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>5</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1000-1500</t>
+          <t>Yes: sleep</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>800-1000</t>
+          <t>work, health</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2023-12-02 08:06:18</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1500-2000</t>
-        </is>
+          <t>2023-12-04 12:17:36</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1000-1500</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>800-1000</t>
+          <t>other</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2023-12-04 12:16:57</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1500-2000</t>
-        </is>
+          <t>2023-12-05 07:53:29</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2000-2500</t>
+          <t>Yes: 5</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1500-2000</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>2023-12-02 08:03:15</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>2-3</t>
-        </is>
-      </c>
-      <c r="C1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D1" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2023-12-02 08:03:15</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2-3</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D2" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2023-12-02 08:06:25</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>5</v>
-      </c>
-      <c r="D3" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2023-12-02 08:06:25</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>5</v>
-      </c>
-      <c r="D4" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2023-12-04 12:17:08</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2-3</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" t="n">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>2023-12-02 08:04:12</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
           <t>4</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2023-12-02 08:04:12</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>3</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2023-12-02 08:06:32</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2023-12-02 08:06:32</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2023-12-04 12:17:15</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>4</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>2023-12-02 08:05:09</t>
-        </is>
-      </c>
-      <c r="B1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>happy, sad</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2023-12-02 08:05:09</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>happy, sad</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2023-12-04 12:17:22</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>3</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>cold, tired, sleepy</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>2023-12-02 08:05:24</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Yes: Sleep</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>finance, personal life</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2023-12-02 08:05:24</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Yes: Sleep</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>finance, personal life</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2023-12-04 11:53:49</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>5</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Yes: sleep</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>work, health</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2023-12-04 12:17:36</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>4</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>other</t>
         </is>
       </c>
     </row>

</xml_diff>